<commit_message>
TuNguyen - refactor script for iOS
</commit_message>
<xml_diff>
--- a/src/test/resources/dataprovider/business_detail/BusinessDetail.xlsx
+++ b/src/test/resources/dataprovider/business_detail/BusinessDetail.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22725"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22801"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FD2456DE-EDB3-4D4D-A07A-3E223DAC772C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E8EDC9B-25C8-45F6-A4E5-05FD8DC85C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Business Type</t>
   </si>
@@ -60,10 +60,7 @@
     <t>Partnership</t>
   </si>
   <si>
-    <t>TIM PENNY ARCHITECTURE &amp; INTERIORS PTY. LTD.</t>
-  </si>
-  <si>
-    <t>Penny Contemporary</t>
+    <t>I.C HILL &amp; L.A HILL &amp; S HILL &amp; R.L JAKINS</t>
   </si>
   <si>
     <t>N/A</t>
@@ -424,7 +421,7 @@
   <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -474,7 +471,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="6">
-        <v>37136594735</v>
+        <v>95488716489</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>10</v>
@@ -483,41 +480,41 @@
         <v>11</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="17" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B4" s="9">
         <v>94330845794</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="10" t="s">
+      <c r="E4" s="11" t="s">
         <v>15</v>
-      </c>
-      <c r="E4" s="11" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B5" s="15">
         <v>17968326471</v>
       </c>
       <c r="C5" s="16" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E5" s="14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update - add more testcase
</commit_message>
<xml_diff>
--- a/src/test/resources/dataprovider/business_detail/BusinessDetail.xlsx
+++ b/src/test/resources/dataprovider/business_detail/BusinessDetail.xlsx
@@ -1,27 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22801"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2E8EDC9B-25C8-45F6-A4E5-05FD8DC85C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="630" yWindow="600" windowWidth="27495" windowHeight="11955" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <definedNames/>
+  <calcPr/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjWZaq1xEWOFXyKWIrXA8F2Q812GA=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId5" roundtripDataSignature="AMtx7mjvrO74kLb6BsHDg2nmQBCjWVbxow=="/>
     </ext>
   </extLst>
 </workbook>
@@ -60,7 +48,7 @@
     <t>Partnership</t>
   </si>
   <si>
-    <t>I.C HILL &amp; L.A HILL &amp; S HILL &amp; R.L JAKINS</t>
+    <t>I.C HILL &amp; S HILL &amp; THE TRUSTEE FOR J H FAMILY TRUST</t>
   </si>
   <si>
     <t>N/A</t>
@@ -87,52 +75,38 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
-    <font>
-      <sz val="11"/>
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <fonts count="6">
+    <font>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <u/>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color theme="10"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF0563C1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="163"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="163"/>
     </font>
   </fonts>
   <fills count="3">
@@ -140,7 +114,7 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="gray125"/>
+      <patternFill patternType="lightGray"/>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -149,14 +123,8 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+  <borders count="3">
+    <border/>
     <border>
       <left style="thin">
         <color rgb="FF000000"/>
@@ -170,58 +138,56 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
-      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="14">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="5" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -411,28 +377,26 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+  <sheetPr>
+    <pageSetUpPr/>
+  </sheetPr>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.875" customWidth="1"/>
-    <col min="2" max="2" width="13.375" customWidth="1"/>
-    <col min="3" max="3" width="38.875" customWidth="1"/>
-    <col min="4" max="5" width="19.75" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="10.38"/>
+    <col customWidth="1" min="2" max="2" width="11.75"/>
+    <col customWidth="1" min="3" max="3" width="34.0"/>
+    <col customWidth="1" min="4" max="5" width="17.25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -449,12 +413,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2">
       <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="3">
-        <v>44004584552</v>
+        <v>4.4004584552E10</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
@@ -466,12 +430,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="19.5" customHeight="1">
+    <row r="3" ht="19.5" customHeight="1">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B3" s="6">
-        <v>95488716489</v>
+        <v>9.5488716489E10</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>10</v>
@@ -483,12 +447,12 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" s="17" t="s">
+    <row r="4">
+      <c r="A4" s="3" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="9">
-        <v>94330845794</v>
+        <v>9.4330845794E10</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>13</v>
@@ -500,28 +464,30 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="12" t="s">
+    <row r="5">
+      <c r="A5" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="15">
-        <v>17968326471</v>
-      </c>
-      <c r="C5" s="16" t="s">
+      <c r="B5" s="9">
+        <v>1.7968326471E10</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D4" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId1" ref="D4"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <printOptions/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>